<commit_message>
- udpated the sheet
</commit_message>
<xml_diff>
--- a/SRS - Copy.xlsx
+++ b/SRS - Copy.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="128">
   <si>
     <t>date</t>
   </si>
@@ -434,6 +434,12 @@
   </si>
   <si>
     <t>I couldn't get room no in the json format.</t>
+  </si>
+  <si>
+    <t>mapping the settings data like the room types role types from the service call</t>
+  </si>
+  <si>
+    <t>we already have service that gives all the settings information /user/settings(get) pls map the response of the room types fetch from the service call not binding the values in the controller if any</t>
   </si>
 </sst>
 </file>
@@ -1402,11 +1408,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H25"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H24" sqref="H24"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1838,6 +1844,27 @@
         <v>42634</v>
       </c>
     </row>
+    <row r="26" spans="1:8" s="2" customFormat="1"/>
+    <row r="27" spans="1:8" ht="75">
+      <c r="A27" s="8">
+        <v>42635</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E27" s="8">
+        <v>42634</v>
+      </c>
+      <c r="F27" s="8">
+        <v>42634</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D25"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1850,7 +1877,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
- udpatd the sheet
</commit_message>
<xml_diff>
--- a/SRS - Copy.xlsx
+++ b/SRS - Copy.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="2"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="data fields" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="141">
   <si>
     <t>date</t>
   </si>
@@ -440,6 +440,46 @@
   </si>
   <si>
     <t>we already have service that gives all the settings information /user/settings(get) pls map the response of the room types fetch from the service call not binding the values in the controller if any</t>
+  </si>
+  <si>
+    <t>select option for check in and booking</t>
+  </si>
+  <si>
+    <t>select option in the check in page so that for each room the user can make check in (in case of same date) or booking (for future) in the check in tab
+Note that this value the value must be either CHECKED-IN or BOOKED as per data coming from server and must be send with key bookingStatus as mentioned in json of /transaction(post)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">db.getCollection('tranctions').aggregate([{ </t>
+  </si>
+  <si>
+    <t xml:space="preserve">        $match : {</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            'roomsDetails.price':100</t>
+  </si>
+  <si>
+    <t xml:space="preserve">            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">         }</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    }])</t>
+  </si>
+  <si>
+    <t>get the price matching with the array of the rooms</t>
+  </si>
+  <si>
+    <t>Note if we want to get data matching key value from the array of objects then we have to use aggregrate</t>
+  </si>
+  <si>
+    <t>if we want to update data in array of objects then we have to use $</t>
+  </si>
+  <si>
+    <t>in case we want to use aggregrate and populate then first we have to get the data from aggregrate and then populate it</t>
+  </si>
+  <si>
+    <t>updated the web service for the get transaction where the parameres are remain the same but the response is different</t>
   </si>
 </sst>
 </file>
@@ -516,7 +556,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -554,10 +594,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1408,11 +1444,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:H27"/>
+  <dimension ref="A1:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A19" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1865,6 +1901,26 @@
         <v>42634</v>
       </c>
     </row>
+    <row r="28" spans="1:8" ht="150">
+      <c r="A28" s="8">
+        <v>42635</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="E28" s="8">
+        <v>42634</v>
+      </c>
+      <c r="F28" s="8">
+        <v>42634</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="D1:D25"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1874,39 +1930,102 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.140625" customWidth="1"/>
-    <col min="3" max="3" width="91.85546875" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="64.140625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="91.85546875" style="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="13" customFormat="1">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:3" s="3" customFormat="1">
+      <c r="A1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="3" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="14">
-        <v>42634</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="8">
+        <v>42634</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="1" t="s">
         <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="B3" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="C4" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="C5" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="C6" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="C7" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="C8" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30">
+      <c r="A10" s="8">
+        <v>42635</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="B11" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30">
+      <c r="A13" s="8">
+        <v>42635</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30">
+      <c r="A15" s="8">
+        <v>42635</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>

</xml_diff>